<commit_message>
Resolviendo el problema de la elimnacion de empleado y agregando el manual de usuarios en el menu de ayudas
</commit_message>
<xml_diff>
--- a/Reportes/ReporteNomina.xlsx
+++ b/Reportes/ReporteNomina.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
   <si>
     <t>ID Empleado</t>
   </si>
@@ -83,97 +83,106 @@
     <t>5</t>
   </si>
   <si>
+    <t xml:space="preserve">Pedro </t>
+  </si>
+  <si>
+    <t>Sanchez</t>
+  </si>
+  <si>
+    <t>6587432</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>Q3,750.00</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>2025-03-31</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Q0.00</t>
+  </si>
+  <si>
+    <t>Q250.00</t>
+  </si>
+  <si>
+    <t>Q93.75</t>
+  </si>
+  <si>
+    <t>Q4,093.75</t>
+  </si>
+  <si>
+    <t>Q185.65</t>
+  </si>
+  <si>
+    <t>Q435.65</t>
+  </si>
+  <si>
+    <t>Q3,658.10</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Giovanni</t>
   </si>
   <si>
     <t>Cifuentes</t>
   </si>
   <si>
-    <t>1234568</t>
+    <t>7894567</t>
+  </si>
+  <si>
+    <t>2025-03-17</t>
+  </si>
+  <si>
+    <t>Q4,000.00</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>1008</t>
+  </si>
+  <si>
+    <t>2025-03-02</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Q4,250.00</t>
+  </si>
+  <si>
+    <t>Q193.20</t>
+  </si>
+  <si>
+    <t>Q4,056.80</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Perez</t>
+  </si>
+  <si>
+    <t>1234567890101</t>
   </si>
   <si>
     <t>2025-03-06</t>
   </si>
   <si>
-    <t>3750.00</t>
-  </si>
-  <si>
-    <t>Activo</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>2025-03-31</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>250.00</t>
-  </si>
-  <si>
-    <t>93.750000000</t>
-  </si>
-  <si>
-    <t>4093.750000000</t>
-  </si>
-  <si>
-    <t>185.6531250000000</t>
-  </si>
-  <si>
-    <t>435.6531250000000</t>
-  </si>
-  <si>
-    <t>3658.0968750000000</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7894567</t>
-  </si>
-  <si>
-    <t>2025-03-17</t>
-  </si>
-  <si>
-    <t>4000.00</t>
-  </si>
-  <si>
-    <t>1008</t>
-  </si>
-  <si>
-    <t>2025-03-02</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>0E-9</t>
-  </si>
-  <si>
-    <t>4250.000000000</t>
-  </si>
-  <si>
-    <t>193.2000000000000</t>
-  </si>
-  <si>
-    <t>4056.8000000000000</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>1234567890101</t>
-  </si>
-  <si>
-    <t>5500.00</t>
+    <t>Q5,500.00</t>
   </si>
   <si>
     <t>1009</t>
@@ -185,19 +194,19 @@
     <t>2</t>
   </si>
   <si>
-    <t>68.749999860</t>
-  </si>
-  <si>
-    <t>5818.749999860</t>
-  </si>
-  <si>
-    <t>281.0456249932380</t>
-  </si>
-  <si>
-    <t>531.0456249932380</t>
-  </si>
-  <si>
-    <t>5287.7043748667620</t>
+    <t>Q68.75</t>
+  </si>
+  <si>
+    <t>Q5,818.75</t>
+  </si>
+  <si>
+    <t>Q281.05</t>
+  </si>
+  <si>
+    <t>Q531.05</t>
+  </si>
+  <si>
+    <t>Q5,287.70</t>
   </si>
   <si>
     <t>1010</t>
@@ -206,16 +215,46 @@
     <t>2025-03-26</t>
   </si>
   <si>
-    <t>46.875000000</t>
-  </si>
-  <si>
-    <t>4046.875000000</t>
-  </si>
-  <si>
-    <t>183.3890625000000</t>
-  </si>
-  <si>
-    <t>3863.4859375000000</t>
+    <t>Q46.88</t>
+  </si>
+  <si>
+    <t>Q4,046.88</t>
+  </si>
+  <si>
+    <t>Q183.39</t>
+  </si>
+  <si>
+    <t>Q3,863.49</t>
+  </si>
+  <si>
+    <t>Gustavo</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>1923546</t>
+  </si>
+  <si>
+    <t>2014-05-19</t>
+  </si>
+  <si>
+    <t>Q8,500.00</t>
+  </si>
+  <si>
+    <t>2011</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>Q8,750.00</t>
+  </si>
+  <si>
+    <t>Q410.55</t>
+  </si>
+  <si>
+    <t>Q8,339.45</t>
   </si>
 </sst>
 </file>
@@ -260,7 +299,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -407,34 +446,34 @@
         <v>39</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>42</v>
-      </c>
       <c r="K3" t="s" s="0">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L3" t="s" s="0">
         <v>32</v>
@@ -443,10 +482,10 @@
         <v>33</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="P3" t="s" s="0">
         <v>32</v>
@@ -461,13 +500,13 @@
         <v>32</v>
       </c>
       <c r="T3" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="U3" t="s" s="0">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="V3" t="s" s="0">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4">
@@ -475,34 +514,34 @@
         <v>31</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L4" t="s" s="0">
         <v>33</v>
@@ -511,10 +550,10 @@
         <v>32</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="P4" t="s" s="0">
         <v>32</v>
@@ -529,13 +568,13 @@
         <v>33</v>
       </c>
       <c r="T4" t="s" s="0">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="U4" t="s" s="0">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="V4" t="s" s="0">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
@@ -561,16 +600,16 @@
         <v>28</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s" s="0">
         <v>27</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L5" t="s" s="0">
         <v>32</v>
@@ -579,10 +618,10 @@
         <v>33</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="P5" t="s" s="0">
         <v>32</v>
@@ -597,13 +636,81 @@
         <v>32</v>
       </c>
       <c r="T5" t="s" s="0">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="U5" t="s" s="0">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="V5" t="s" s="0">
-        <v>67</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="Q6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="S6" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="T6" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="U6" t="s" s="0">
+        <v>79</v>
+      </c>
+      <c r="V6" t="s" s="0">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Subiendo el nuevo frontend
</commit_message>
<xml_diff>
--- a/Reportes/ReporteNomina.xlsx
+++ b/Reportes/ReporteNomina.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="83">
   <si>
     <t>ID Empleado</t>
   </si>
@@ -242,19 +242,25 @@
     <t>Q8,500.00</t>
   </si>
   <si>
-    <t>2011</t>
+    <t>3011</t>
   </si>
   <si>
     <t>2025-05-30</t>
   </si>
   <si>
-    <t>Q8,750.00</t>
-  </si>
-  <si>
-    <t>Q410.55</t>
-  </si>
-  <si>
-    <t>Q8,339.45</t>
+    <t>Q500.00</t>
+  </si>
+  <si>
+    <t>Q106.25</t>
+  </si>
+  <si>
+    <t>Q9,356.25</t>
+  </si>
+  <si>
+    <t>Q439.83</t>
+  </si>
+  <si>
+    <t>Q8,916.42</t>
   </si>
 </sst>
 </file>
@@ -677,19 +683,19 @@
         <v>75</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="M6" t="s" s="0">
         <v>33</v>
       </c>
       <c r="N6" t="s" s="0">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="O6" t="s" s="0">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="P6" t="s" s="0">
         <v>32</v>
@@ -704,13 +710,13 @@
         <v>32</v>
       </c>
       <c r="T6" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="U6" t="s" s="0">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="V6" t="s" s="0">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>